<commit_message>
Update VIP Card BOM
</commit_message>
<xml_diff>
--- a/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
+++ b/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/AVIELF2-VIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{44D56BEF-7FC0-8047-A3D0-A0DF5FC882B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D561D24-7863-804B-82B2-D8A0C28E6884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="13060" windowWidth="26840" windowHeight="15940"/>
+    <workbookView xWindow="15780" yWindow="2880" windowWidth="39240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVIELF2-VIP" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>C1, C2, C3</t>
   </si>
@@ -58,18 +58,12 @@
     <t>/Q LED</t>
   </si>
   <si>
-    <t>Device:LED</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
     <t>D</t>
   </si>
   <si>
-    <t>Device:D</t>
-  </si>
-  <si>
     <t>1=K 2=A</t>
   </si>
   <si>
@@ -127,18 +121,9 @@
     <t>2N3906</t>
   </si>
   <si>
-    <t>Transistor_BJT:2N3906</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pub/Collateral/2N3906-D.PDF</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
-    <t>Device:R_Small_US</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -172,12 +157,6 @@
     <t>3949-OWS-131845LA-8D-ND</t>
   </si>
   <si>
-    <t>Device:Speaker</t>
-  </si>
-  <si>
-    <t>Switch:SW_Push</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -190,12 +169,6 @@
     <t>NE555</t>
   </si>
   <si>
-    <t>1_Josh_lib:ICM7555xP</t>
-  </si>
-  <si>
-    <t>http://www.intersil.com/content/dam/Intersil/documents/icm7/icm7555-56.pdf</t>
-  </si>
-  <si>
     <t>QUANTITY</t>
   </si>
   <si>
@@ -235,17 +208,119 @@
     <t>4-Bit Latched/4-to-16 Line Decoders</t>
   </si>
   <si>
-    <t>Not in stock at DigiKey or Mouser. May need to purchase from Jameco or Ebay</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/ole-wolff-electronics-inc/OWS-131845LA-8D/17636884</t>
+  </si>
+  <si>
+    <t>Not in stock at DigiKey or Mouser. Limited supply at Jameco: https://www.jameco.com/webapp/wcs/stores/servlet/ProductDisplay?langId=-1&amp;storeId=10001&amp;catalogId=10001&amp;productId=2290471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Ohms Microspeaker Speaker 1 W 10 Hz ~ 10 kHz </t>
+  </si>
+  <si>
+    <t>Cherry type keyboard switch (Amazon 30 piece set)</t>
+  </si>
+  <si>
+    <t>Amazon: https://www.amazon.ca/dp/B0BXZXZX74</t>
+  </si>
+  <si>
+    <t>555 Type, Timer/Oscillator (Single) IC 100kHz 8-PDIP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/NE555P/277057</t>
+  </si>
+  <si>
+    <t>0.1uf Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>0.1uf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/kemet/C320C104K5R5TA7317/6562447</t>
+  </si>
+  <si>
+    <t>IC's</t>
+  </si>
+  <si>
+    <t>Semiconductors</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/comchip-technology/2N3906-G/9477908</t>
+  </si>
+  <si>
+    <t>Bipolar (BJT) Transistor PNP 40 V 200 mA 250MHz Through Hole TO-92</t>
+  </si>
+  <si>
+    <t>5mm LED Diffused: Red</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/liteon/LTL2R3KRD-EM/2675133</t>
+  </si>
+  <si>
+    <t>1N914</t>
+  </si>
+  <si>
+    <t>Diode 100 V 200mA Through Hole DO-35</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/onsemi/1N914/978749</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Connectors</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT330R/1741399 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT10K0/1741265 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT1K00/1741314</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT750K/1741503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">750 kOhms Carbon Film Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 kOhms Carbon Film Resistor  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 kOhms Carbon Film Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7 kOhms Carbon Film Resistor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Ohms Carbon Film Resistor </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT4K70/1741428</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CF14JT10R0/1741276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330 Ohms Carbon Film Resistor </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,6 +462,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -737,7 +824,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -748,6 +835,20 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1103,73 +1204,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" customWidth="1"/>
     <col min="5" max="5" width="70.6640625" customWidth="1"/>
+    <col min="6" max="6" width="100" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1177,90 +1269,59 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
+        <v>59</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
+        <v>67</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1268,16 +1329,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1285,81 +1346,66 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2</v>
-      </c>
+      <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>2</v>
@@ -1370,67 +1416,38 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3">
-        <v>330</v>
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>2</v>
+      <c r="A18" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1438,33 +1455,35 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" t="s">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="9">
+        <v>330</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" t="s">
-        <v>2</v>
+        <v>34</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1472,16 +1491,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="3">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" t="s">
-        <v>2</v>
+        <v>90</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1489,33 +1508,33 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" t="s">
-        <v>2</v>
+        <v>93</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1523,56 +1542,205 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+      <c r="C24" s="3">
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" t="s">
-        <v>57</v>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F25" r:id="rId1"/>
-    <hyperlink ref="F22" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F27" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E30" r:id="rId3" display="https://www.amazon.ca/dp/B0BXZXZX74" xr:uid="{348F9A02-6ABA-7C4D-8788-10FD7C8F8948}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{B7E2300A-3A35-2F47-82EA-BA71C3D536FF}"/>
+    <hyperlink ref="F13" r:id="rId5" xr:uid="{6C391331-F58F-594D-BE25-6A53B377B9BB}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{D9654F22-5145-F342-9213-12EEA899C91C}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{29196CB2-A66B-9D4A-8CC9-40EDAF945AA8}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{16DE85FC-75EE-7D4E-97BE-A2D251817B61}"/>
+    <hyperlink ref="F19" r:id="rId9" xr:uid="{3A3CD688-653E-754B-A20A-B98D7DB105B4}"/>
+    <hyperlink ref="F20" r:id="rId10" xr:uid="{89F71375-8539-8D48-B2C3-BF8DC1C05EA1}"/>
+    <hyperlink ref="F22" r:id="rId11" xr:uid="{AF168BCD-5770-834F-BFEE-39C6924E4A37}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{09EC3549-D471-AE49-9897-33FC38298809}"/>
+    <hyperlink ref="F23" r:id="rId13" xr:uid="{87E20272-D533-2345-A4E6-ADD997D5AAEF}"/>
+    <hyperlink ref="F24" r:id="rId14" xr:uid="{0A2A6153-4850-D846-97E6-DE18ECEC74F6}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Sync Local VIP Card BOM
</commit_message>
<xml_diff>
--- a/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
+++ b/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/AVIELF2-VIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{591ED606-D74B-284D-B6C3-50F1C950AF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B6534F8-B938-1D47-A676-8ED2671A6F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="2880" windowWidth="39240" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15780" yWindow="2880" windowWidth="39020" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AVIELF2-VIP" sheetId="1" r:id="rId1"/>
+    <sheet name="Digikey.ca" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update all schematics, images and gerbers
</commit_message>
<xml_diff>
--- a/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
+++ b/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/AVIELF2-VIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B6534F8-B938-1D47-A676-8ED2671A6F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679213E9-6C04-3F44-8011-9A94A0F88A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15780" yWindow="2880" windowWidth="39020" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update VIP Card BOM Add Mouser
</commit_message>
<xml_diff>
--- a/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
+++ b/notes/AVIELF2-VIP/AVIELF2-VIP-BOM.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/AVIELF2-VIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ADC77D-B6B3-6D42-A8BC-998CFDF1A850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64E1721-E12C-A040-9FB5-9014F62C8496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="3540" windowWidth="26940" windowHeight="18640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26280" yWindow="3800" windowWidth="26940" windowHeight="18640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey.ca" sheetId="1" r:id="rId1"/>
     <sheet name="Digikey.com" sheetId="2" r:id="rId2"/>
+    <sheet name="Mouser.ca" sheetId="3" r:id="rId3"/>
+    <sheet name="Mouser.com" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="157">
   <si>
     <t>C1, C2, C3</t>
   </si>
@@ -378,6 +380,120 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PREC040SAAN-RC/2774814</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/CD4512BE?qs=tJ5HNKWh3OVRU7x0rQr1%2FQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/NE555P?qs=rkhjVJ6%2F3EIf4CWgjIKuKQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi-Fairchild/2N3906BU?qs=iN0KuJO79Kbn9o7a2lB4uA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/c/optoelectronics/led-lighting/led-emitters/standard-leds-through-hole/?q=5mm%20LED&amp;package%20%2F%20case=T-1%203%2F4%20%285%20mm%29</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/onsemi-Fairchild/1N914B?qs=sGAEpiMZZMtbRapU8LlZDzCgIkNleXIZjCSZIvAdjSc%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Murata-Electronics/RCER71H104K0K1H03B?qs=Zt%252BKPUOg4of53jbypBpoRQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECE-A1VKA100B?qs=sGAEpiMZZMsh%252B1woXyUXj%2FCjDN34kA%252BzNH8IV1070Pk%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Vishay/564R75GAT47?qs=sGAEpiMZZMuMW9TJLBQkXggNKKPLOSPRfo922S%252BB54s%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/860010572001?qs=0KOYDY2FL2%252BYl5%252BFHccj0w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECE-A1VKS4R7I?qs=rMMd5vBiahonFjmaaaZZoQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Panasonic/ECA-1HEN2R2?qs=tfZGHB2PWd2eLhFRhqLHwQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT330R?qs=FESYatJ8odL8jgcbJiLESA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT10K0?qs=FESYatJ8odJcEE4HXxUVCA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/RNF14BTC750K?qs=IPgv5n7u5Qb6R6ieppNtJg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/CF14JT1K00?qs=FESYatJ8odLLAkjsom%2FJYQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/RNMF14FTC4K70?qs=FESYatJ8odJq0RyP%2FuvZgQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/SEI-Stackpole/RNMF14FTC10R0?qs=FESYatJ8odJTss10hMkuIw%3D%3D</t>
+  </si>
+  <si>
+    <t>Not available at Mouser: https://www.digikey.ca/en/products/detail/ole-wolff-electronics-inc/OWS-131845LA-8D/17636884</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Amphenol-FCI/68691-440HLF?qs=cPwqfQhQFYMYN3UF9G02MQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/CD4512BE?qs=tJ5HNKWh3OVRU7x0rQr1%2FQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Texas-Instruments/NE555P?qs=rkhjVJ6%2F3EIf4CWgjIKuKQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/onsemi-Fairchild/2N3906BU?qs=iN0KuJO79Kbn9o7a2lB4uA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/c/optoelectronics/led-lighting/led-emitters/standard-leds-through-hole/?q=5mm%20LED&amp;package%20%2F%20case=T-1%203%2F4%20%285%20mm%29</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/onsemi-Fairchild/1N914B?qs=sGAEpiMZZMtbRapU8LlZDzCgIkNleXIZjCSZIvAdjSc%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Murata-Electronics/RCER71H104K0K1H03B?qs=Zt%252BKPUOg4of53jbypBpoRQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Vishay/564R75GAT47?qs=sGAEpiMZZMuMW9TJLBQkXggNKKPLOSPRfo922S%252BB54s%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/860010572001?qs=0KOYDY2FL2%252BYl5%252BFHccj0w%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ECE-A1VKS4R7I?qs=rMMd5vBiahonFjmaaaZZoQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ECA-1HEN2R2?qs=tfZGHB2PWd2eLhFRhqLHwQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panasonic/ECE-A1VKA100B?qs=sGAEpiMZZMsh%252B1woXyUXj%2FCjDN34kA%252BzNH8IV1070Pk%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT330R?qs=FESYatJ8odL8jgcbJiLESA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT10K0?qs=FESYatJ8odJcEE4HXxUVCA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/RNF14BTC750K?qs=IPgv5n7u5Qb6R6ieppNtJg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CF14JT1K00?qs=FESYatJ8odLLAkjsom%2FJYQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/RNMF14FTC4K70?qs=FESYatJ8odJq0RyP%2FuvZgQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/RNMF14FTC10R0?qs=FESYatJ8odJTss10hMkuIw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Amphenol-FCI/68691-440HLF?qs=cPwqfQhQFYMYN3UF9G02MQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Not available at Mouser: https://www.digikey.com/en/products/detail/ole-wolff-electronics-inc/OWS-131845LA-8D/17636884</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B6ACC2-CB1B-6047-AB8D-1F769D46FBAD}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2297,4 +2413,1036 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE175B89-2DE0-C244-892B-0F2BF411D57C}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="6" max="6" width="94" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7">
+        <v>330</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{ECEBBA35-14CB-4F47-A6F3-712F4571017D}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{B9FE0927-D8D9-844B-9A0D-149F639FE712}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{51643936-8B4A-D249-8F36-98366E08BEE2}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{9B52C2FA-CEB6-6A43-B24D-6608F930698C}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{3B89C9F7-1792-E148-A64A-DA4DFDC02231}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{047D428C-83ED-0F4B-80A0-2CA2EECA14DD}"/>
+    <hyperlink ref="F14" r:id="rId7" xr:uid="{0CFEE1D2-07EE-5C49-8888-A6FEBD42703B}"/>
+    <hyperlink ref="F15" r:id="rId8" xr:uid="{DF0C68FD-B2CA-0F48-B87E-EAC85592E0D0}"/>
+    <hyperlink ref="F17" r:id="rId9" xr:uid="{6DF97703-5B7F-4246-9FEE-8C6970904DD3}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{4C1EDA69-2AC6-1C47-AFE2-74F44F884D96}"/>
+    <hyperlink ref="E29" r:id="rId11" display="https://www.digikey.ca/en/products/detail/ole-wolff-electronics-inc/OWS-131845LA-8D/17636884" xr:uid="{3804F1B8-9C6F-DC43-A756-C029F19A6E1E}"/>
+    <hyperlink ref="E32" r:id="rId12" display="https://www.amazon.ca/dp/B0BXZXZX74" xr:uid="{37F82DCA-2637-324A-B40F-DC0422F2F469}"/>
+    <hyperlink ref="F22" r:id="rId13" xr:uid="{DE2C1A05-6EC3-8948-AE47-89CC4B7D36FE}"/>
+    <hyperlink ref="F24" r:id="rId14" xr:uid="{262EE825-7483-324B-B257-DC16964ED3A4}"/>
+    <hyperlink ref="F23" r:id="rId15" xr:uid="{29DF3991-0815-BA43-A0BB-4B8368FBDF38}"/>
+    <hyperlink ref="F25" r:id="rId16" xr:uid="{AD62DD9F-74F9-004F-905D-661A5542E3DD}"/>
+    <hyperlink ref="F26" r:id="rId17" xr:uid="{F25A459C-1145-1849-9160-A7A5684F4E50}"/>
+    <hyperlink ref="F35" r:id="rId18" xr:uid="{7D97552C-CB31-4647-B594-7C4CCDFCE0A7}"/>
+    <hyperlink ref="F36" r:id="rId19" xr:uid="{A7C8D6A2-2DA7-C045-A03E-AC8F40C2ACCE}"/>
+    <hyperlink ref="F18" r:id="rId20" xr:uid="{13AA782D-1A6E-B447-B8F1-4E12048C96DF}"/>
+    <hyperlink ref="F21" r:id="rId21" xr:uid="{61042C3D-0D4D-CB40-B94C-2DAFAC21A2A2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE79C91-1F1D-BA42-946F-CAD8E1E78057}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="42.1640625" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" customWidth="1"/>
+    <col min="6" max="6" width="94" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="7">
+        <v>330</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{9840ABFA-2A62-0445-AFC3-C1CB2294C348}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{2DD1AF70-2A55-4045-BD41-6462F8012C06}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{5E7179F0-E8C1-A04D-81BE-DF397058A7CC}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{72E0440F-6DE8-A04F-9733-30121A4A9472}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{542BFAC3-7A3C-BE4A-B8B3-8A4243CF1E52}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{92588B9C-0D32-0A42-8EA9-8DEE4493E7F2}"/>
+    <hyperlink ref="F14" r:id="rId7" xr:uid="{DF1D6580-A906-8143-B519-8D19F092EB19}"/>
+    <hyperlink ref="F15" r:id="rId8" xr:uid="{24189679-39E9-A445-A04E-FB85C9529EC6}"/>
+    <hyperlink ref="F17" r:id="rId9" xr:uid="{43AE9D92-53CA-8446-97FC-1A5042CCB868}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{423CDFB5-602E-524D-A9E4-89392C1A70A7}"/>
+    <hyperlink ref="E29" r:id="rId11" display="https://www.digikey.ca/en/products/detail/ole-wolff-electronics-inc/OWS-131845LA-8D/17636884" xr:uid="{066FD51A-DC9F-ED42-AF03-2152FB8B94D0}"/>
+    <hyperlink ref="E32" r:id="rId12" display="https://www.amazon.ca/dp/B0BXZXZX74" xr:uid="{C7745636-9CF2-4942-B2EF-6D59821B2055}"/>
+    <hyperlink ref="F22" r:id="rId13" xr:uid="{A3CB7498-02B7-AF4E-B864-506232D877DA}"/>
+    <hyperlink ref="F24" r:id="rId14" xr:uid="{68A16E04-F6F9-4044-A28C-2A47BFCCCBC3}"/>
+    <hyperlink ref="F23" r:id="rId15" xr:uid="{17DF3913-9258-3345-A1B4-2293D987C54B}"/>
+    <hyperlink ref="F25" r:id="rId16" xr:uid="{5673BCE3-002D-6E4F-9055-793DCF24EA4C}"/>
+    <hyperlink ref="F26" r:id="rId17" xr:uid="{40566C36-AAB7-0E4B-ACC3-E2912F6653E4}"/>
+    <hyperlink ref="F35" r:id="rId18" xr:uid="{7AA08553-ED03-2F47-BA32-784A37B3B255}"/>
+    <hyperlink ref="F36" r:id="rId19" xr:uid="{3DFBD92A-9335-304E-87E0-5806652576C0}"/>
+    <hyperlink ref="F18" r:id="rId20" xr:uid="{9ABFEC79-F22B-6F4E-934A-24D1059398F3}"/>
+    <hyperlink ref="F21" r:id="rId21" xr:uid="{A8E896DF-A1F2-A64D-B3FF-2ABE4F5DCBE9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>